<commit_message>
xóa những thứ linh tinh add project Moblie
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoachThucHienDACS.xlsx
+++ b/TaiLieu/KeHoachThucHienDACS.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Nhóm US" sheetId="1" r:id="rId1"/>
+    <sheet name="Nhóm US Cũ" sheetId="1" r:id="rId1"/>
+    <sheet name="Mới" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="97">
   <si>
     <t>STT</t>
   </si>
@@ -216,13 +217,112 @@
   </si>
   <si>
     <t>14/5 - 20/502020</t>
+  </si>
+  <si>
+    <t>Kiểm thử phần mềm</t>
+  </si>
+  <si>
+    <t>Viết báo sường báo cáo + hoàn thành báo váp app windows</t>
+  </si>
+  <si>
+    <t>Tìm hiểu nền tảng mobile - Xamarin.Form</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về web - HTML, CSS, JS</t>
+  </si>
+  <si>
+    <t>Viết báo cáo sơ việc về web</t>
+  </si>
+  <si>
+    <t>Lên danh sách trigger + procduct cần thiết cho web</t>
+  </si>
+  <si>
+    <t>Viết báo cáo sơ việc về android</t>
+  </si>
+  <si>
+    <t>Tìm Hiểu ASP.NET mô hình MVC</t>
+  </si>
+  <si>
+    <t>Phác thảo sơ lược giao diện web</t>
+  </si>
+  <si>
+    <t>Xử lý liên kết giữa Domain - hosting - project</t>
+  </si>
+  <si>
+    <t>Tìm Hiểu Xamarin.Form</t>
+  </si>
+  <si>
+    <t>Phác thảo sơ lược giao diện app(android)</t>
+  </si>
+  <si>
+    <t>App Mobile</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Đăng Nhập</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Thiết kế sườn App</t>
+  </si>
+  <si>
+    <t>2/4 - 8/4/2020</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>APP Moblie</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Home</t>
+  </si>
+  <si>
+    <t>Thiết kế trang chuyên cần + Lỗi vi phạm +TKB</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module thông tin HS</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Thông Tin GV</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Xem diểm, hạnh kiểm</t>
+  </si>
+  <si>
+    <t>Code Module Xem điểm + Hạnh Kiểm</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module Xin phép nghỉ học</t>
+  </si>
+  <si>
+    <t>Code Module xem ngày nghỉ</t>
+  </si>
+  <si>
+    <t>Code Module đăng ký nghỉ học có phép</t>
+  </si>
+  <si>
+    <t>Thiết kế + code module xem đánh giá HS</t>
+  </si>
+  <si>
+    <t>Kiểm thử APP + fix Lỗi</t>
+  </si>
+  <si>
+    <t>Hoàng làm 50%</t>
+  </si>
+  <si>
+    <t>Phong làm 50%</t>
+  </si>
+  <si>
+    <t>Hoàng làm 100%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,16 +365,42 @@
       <family val="1"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -759,11 +885,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -858,80 +1060,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1212,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
@@ -1232,56 +1548,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
     </row>
     <row r="14" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="I14" s="51" t="s">
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="I14" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1329,10 +1645,10 @@
       <c r="E17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="52">
         <v>1</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="55" t="s">
         <v>52</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1341,7 +1657,7 @@
       <c r="L17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="65">
+      <c r="M17" s="45">
         <v>1</v>
       </c>
       <c r="N17" s="3"/>
@@ -1359,15 +1675,15 @@
       <c r="E18" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="43"/>
-      <c r="J18" s="46"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="56"/>
       <c r="K18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L18" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="66">
+      <c r="M18" s="46">
         <v>1</v>
       </c>
       <c r="N18" s="6"/>
@@ -1385,61 +1701,61 @@
       <c r="E19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="49" t="s">
+      <c r="I19" s="53"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="48" t="s">
         <v>9</v>
       </c>
       <c r="L19" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="66">
+      <c r="M19" s="46">
         <v>1</v>
       </c>
       <c r="N19" s="6"/>
     </row>
     <row r="20" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I20" s="43"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="49"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="48"/>
       <c r="L20" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="M20" s="66">
+      <c r="M20" s="46">
         <v>1</v>
       </c>
       <c r="N20" s="6"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I21" s="43"/>
-      <c r="J21" s="46"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="56"/>
       <c r="K21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L21" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="66">
+      <c r="M21" s="46">
         <v>1</v>
       </c>
       <c r="N21" s="6"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I22" s="43"/>
-      <c r="J22" s="46"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="56"/>
       <c r="K22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L22" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="66">
+      <c r="M22" s="46">
         <v>1</v>
       </c>
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="56"/>
+      <c r="I23" s="54"/>
       <c r="J23" s="57"/>
       <c r="K23" s="15" t="s">
         <v>53</v>
@@ -1447,16 +1763,16 @@
       <c r="L23" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="67">
+      <c r="M23" s="47">
         <v>1</v>
       </c>
       <c r="N23" s="16"/>
     </row>
     <row r="24" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I24" s="52">
+      <c r="I24" s="58">
         <v>2</v>
       </c>
-      <c r="J24" s="54" t="s">
+      <c r="J24" s="60" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="10" t="s">
@@ -1469,8 +1785,8 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I25" s="43"/>
-      <c r="J25" s="46"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="56"/>
       <c r="K25" s="4" t="s">
         <v>15</v>
       </c>
@@ -1481,8 +1797,8 @@
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I26" s="43"/>
-      <c r="J26" s="46"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="56"/>
       <c r="K26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1493,8 +1809,8 @@
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I27" s="43"/>
-      <c r="J27" s="46"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1505,8 +1821,8 @@
       <c r="N27" s="6"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I28" s="43"/>
-      <c r="J28" s="46"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="56"/>
       <c r="K28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1517,9 +1833,9 @@
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I29" s="43"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="49" t="s">
+      <c r="I29" s="53"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="48" t="s">
         <v>20</v>
       </c>
       <c r="L29" s="33" t="s">
@@ -1529,9 +1845,9 @@
       <c r="N29" s="6"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I30" s="43"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="49"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="48"/>
       <c r="L30" s="33" t="s">
         <v>10</v>
       </c>
@@ -1539,9 +1855,9 @@
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I31" s="53"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="60"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="49"/>
       <c r="L31" s="36" t="s">
         <v>11</v>
       </c>
@@ -1549,13 +1865,13 @@
       <c r="N31" s="9"/>
     </row>
     <row r="32" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I32" s="42">
+      <c r="I32" s="62">
         <v>3</v>
       </c>
-      <c r="J32" s="45" t="s">
+      <c r="J32" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="K32" s="48" t="s">
+      <c r="K32" s="66" t="s">
         <v>21</v>
       </c>
       <c r="L32" s="32" t="s">
@@ -1565,9 +1881,9 @@
       <c r="N32" s="14"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I33" s="43"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="49"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="48"/>
       <c r="L33" s="33" t="s">
         <v>10</v>
       </c>
@@ -1575,9 +1891,9 @@
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I34" s="43"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="49"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="33" t="s">
         <v>11</v>
       </c>
@@ -1585,8 +1901,8 @@
       <c r="N34" s="6"/>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I35" s="43"/>
-      <c r="J35" s="46"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="56"/>
       <c r="K35" s="4" t="s">
         <v>22</v>
       </c>
@@ -1597,8 +1913,8 @@
       <c r="N35" s="6"/>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I36" s="43"/>
-      <c r="J36" s="46"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="56"/>
       <c r="K36" s="4" t="s">
         <v>25</v>
       </c>
@@ -1609,7 +1925,7 @@
       <c r="N36" s="6"/>
     </row>
     <row r="37" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I37" s="56"/>
+      <c r="I37" s="54"/>
       <c r="J37" s="57"/>
       <c r="K37" s="15" t="s">
         <v>28</v>
@@ -1621,10 +1937,10 @@
       <c r="N37" s="16"/>
     </row>
     <row r="38" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I38" s="52">
+      <c r="I38" s="58">
         <v>4</v>
       </c>
-      <c r="J38" s="54" t="s">
+      <c r="J38" s="60" t="s">
         <v>55</v>
       </c>
       <c r="K38" s="10" t="s">
@@ -1637,8 +1953,8 @@
       <c r="N38" s="12"/>
     </row>
     <row r="39" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I39" s="43"/>
-      <c r="J39" s="46"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="56"/>
       <c r="K39" s="4" t="s">
         <v>24</v>
       </c>
@@ -1649,8 +1965,8 @@
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I40" s="43"/>
-      <c r="J40" s="46"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="56"/>
       <c r="K40" s="4" t="s">
         <v>26</v>
       </c>
@@ -1661,8 +1977,8 @@
       <c r="N40" s="6"/>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I41" s="43"/>
-      <c r="J41" s="46"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="56"/>
       <c r="K41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1673,8 +1989,8 @@
       <c r="N41" s="6"/>
     </row>
     <row r="42" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I42" s="43"/>
-      <c r="J42" s="46"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="56"/>
       <c r="K42" s="4" t="s">
         <v>29</v>
       </c>
@@ -1685,8 +2001,8 @@
       <c r="N42" s="6"/>
     </row>
     <row r="43" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I43" s="53"/>
-      <c r="J43" s="55"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="61"/>
       <c r="K43" s="8" t="s">
         <v>30</v>
       </c>
@@ -1697,10 +2013,10 @@
       <c r="N43" s="9"/>
     </row>
     <row r="44" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I44" s="42">
+      <c r="I44" s="62">
         <v>5</v>
       </c>
-      <c r="J44" s="45" t="s">
+      <c r="J44" s="63" t="s">
         <v>56</v>
       </c>
       <c r="K44" s="13" t="s">
@@ -1713,8 +2029,8 @@
       <c r="N44" s="14"/>
     </row>
     <row r="45" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I45" s="43"/>
-      <c r="J45" s="46"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="56"/>
       <c r="K45" s="41" t="s">
         <v>32</v>
       </c>
@@ -1725,8 +2041,8 @@
       <c r="N45" s="6"/>
     </row>
     <row r="46" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I46" s="43"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="56"/>
       <c r="K46" s="4" t="s">
         <v>33</v>
       </c>
@@ -1737,7 +2053,7 @@
       <c r="N46" s="6"/>
     </row>
     <row r="47" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I47" s="56"/>
+      <c r="I47" s="54"/>
       <c r="J47" s="57"/>
       <c r="K47" s="15" t="s">
         <v>34</v>
@@ -1749,10 +2065,10 @@
       <c r="N47" s="16"/>
     </row>
     <row r="48" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I48" s="52">
+      <c r="I48" s="58">
         <v>6</v>
       </c>
-      <c r="J48" s="54" t="s">
+      <c r="J48" s="60" t="s">
         <v>57</v>
       </c>
       <c r="K48" s="10" t="s">
@@ -1765,8 +2081,8 @@
       <c r="N48" s="12"/>
     </row>
     <row r="49" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I49" s="43"/>
-      <c r="J49" s="46"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="56"/>
       <c r="K49" s="4" t="s">
         <v>36</v>
       </c>
@@ -1777,8 +2093,8 @@
       <c r="N49" s="6"/>
     </row>
     <row r="50" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I50" s="43"/>
-      <c r="J50" s="46"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="56"/>
       <c r="K50" s="4" t="s">
         <v>37</v>
       </c>
@@ -1789,8 +2105,8 @@
       <c r="N50" s="6"/>
     </row>
     <row r="51" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I51" s="53"/>
-      <c r="J51" s="55"/>
+      <c r="I51" s="59"/>
+      <c r="J51" s="61"/>
       <c r="K51" s="8" t="s">
         <v>38</v>
       </c>
@@ -1801,13 +2117,13 @@
       <c r="N51" s="9"/>
     </row>
     <row r="52" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I52" s="42">
-        <v>7</v>
-      </c>
-      <c r="J52" s="45" t="s">
+      <c r="I52" s="62">
+        <v>7</v>
+      </c>
+      <c r="J52" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="K52" s="48" t="s">
+      <c r="K52" s="66" t="s">
         <v>39</v>
       </c>
       <c r="L52" s="32" t="s">
@@ -1817,9 +2133,9 @@
       <c r="N52" s="14"/>
     </row>
     <row r="53" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I53" s="43"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="49"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="48"/>
       <c r="L53" s="33" t="s">
         <v>10</v>
       </c>
@@ -1827,9 +2143,9 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I54" s="56"/>
+      <c r="I54" s="54"/>
       <c r="J54" s="57"/>
-      <c r="K54" s="58"/>
+      <c r="K54" s="69"/>
       <c r="L54" s="37" t="s">
         <v>11</v>
       </c>
@@ -1837,13 +2153,13 @@
       <c r="N54" s="16"/>
     </row>
     <row r="55" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I55" s="52">
+      <c r="I55" s="58">
         <v>8</v>
       </c>
-      <c r="J55" s="54" t="s">
+      <c r="J55" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="K55" s="59" t="s">
+      <c r="K55" s="70" t="s">
         <v>40</v>
       </c>
       <c r="L55" s="35" t="s">
@@ -1853,9 +2169,9 @@
       <c r="N55" s="12"/>
     </row>
     <row r="56" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I56" s="43"/>
-      <c r="J56" s="46"/>
-      <c r="K56" s="49"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="48"/>
       <c r="L56" s="33" t="s">
         <v>10</v>
       </c>
@@ -1863,9 +2179,9 @@
       <c r="N56" s="6"/>
     </row>
     <row r="57" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I57" s="43"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="49"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="48"/>
       <c r="L57" s="33" t="s">
         <v>11</v>
       </c>
@@ -1873,8 +2189,8 @@
       <c r="N57" s="6"/>
     </row>
     <row r="58" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I58" s="43"/>
-      <c r="J58" s="46"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="56"/>
       <c r="K58" s="4" t="s">
         <v>41</v>
       </c>
@@ -1885,8 +2201,8 @@
       <c r="N58" s="6"/>
     </row>
     <row r="59" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I59" s="43"/>
-      <c r="J59" s="46"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="56"/>
       <c r="K59" s="4" t="s">
         <v>23</v>
       </c>
@@ -1897,8 +2213,8 @@
       <c r="N59" s="6"/>
     </row>
     <row r="60" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I60" s="53"/>
-      <c r="J60" s="55"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="61"/>
       <c r="K60" s="8" t="s">
         <v>24</v>
       </c>
@@ -1909,10 +2225,10 @@
       <c r="N60" s="9"/>
     </row>
     <row r="61" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I61" s="42">
+      <c r="I61" s="62">
         <v>9</v>
       </c>
-      <c r="J61" s="45" t="s">
+      <c r="J61" s="63" t="s">
         <v>60</v>
       </c>
       <c r="K61" s="13" t="s">
@@ -1925,8 +2241,8 @@
       <c r="N61" s="14"/>
     </row>
     <row r="62" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I62" s="43"/>
-      <c r="J62" s="46"/>
+      <c r="I62" s="53"/>
+      <c r="J62" s="56"/>
       <c r="K62" s="4" t="s">
         <v>26</v>
       </c>
@@ -1937,8 +2253,8 @@
       <c r="N62" s="6"/>
     </row>
     <row r="63" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I63" s="43"/>
-      <c r="J63" s="46"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="56"/>
       <c r="K63" s="4" t="s">
         <v>27</v>
       </c>
@@ -1949,8 +2265,8 @@
       <c r="N63" s="6"/>
     </row>
     <row r="64" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I64" s="43"/>
-      <c r="J64" s="46"/>
+      <c r="I64" s="53"/>
+      <c r="J64" s="56"/>
       <c r="K64" s="4" t="s">
         <v>28</v>
       </c>
@@ -1961,8 +2277,8 @@
       <c r="N64" s="6"/>
     </row>
     <row r="65" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I65" s="43"/>
-      <c r="J65" s="46"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="56"/>
       <c r="K65" s="4" t="s">
         <v>29</v>
       </c>
@@ -1973,7 +2289,7 @@
       <c r="N65" s="6"/>
     </row>
     <row r="66" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I66" s="56"/>
+      <c r="I66" s="54"/>
       <c r="J66" s="57"/>
       <c r="K66" s="15" t="s">
         <v>30</v>
@@ -1985,10 +2301,10 @@
       <c r="N66" s="16"/>
     </row>
     <row r="67" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I67" s="52">
-        <v>10</v>
-      </c>
-      <c r="J67" s="54" t="s">
+      <c r="I67" s="58">
+        <v>10</v>
+      </c>
+      <c r="J67" s="60" t="s">
         <v>61</v>
       </c>
       <c r="K67" s="10" t="s">
@@ -2001,8 +2317,8 @@
       <c r="N67" s="12"/>
     </row>
     <row r="68" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I68" s="43"/>
-      <c r="J68" s="46"/>
+      <c r="I68" s="53"/>
+      <c r="J68" s="56"/>
       <c r="K68" s="17" t="s">
         <v>32</v>
       </c>
@@ -2013,8 +2329,8 @@
       <c r="N68" s="6"/>
     </row>
     <row r="69" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I69" s="43"/>
-      <c r="J69" s="46"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="56"/>
       <c r="K69" s="4" t="s">
         <v>33</v>
       </c>
@@ -2025,8 +2341,8 @@
       <c r="N69" s="6"/>
     </row>
     <row r="70" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I70" s="53"/>
-      <c r="J70" s="55"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="61"/>
       <c r="K70" s="8" t="s">
         <v>34</v>
       </c>
@@ -2037,10 +2353,10 @@
       <c r="N70" s="9"/>
     </row>
     <row r="71" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I71" s="52">
-        <v>11</v>
-      </c>
-      <c r="J71" s="54" t="s">
+      <c r="I71" s="58">
+        <v>11</v>
+      </c>
+      <c r="J71" s="60" t="s">
         <v>62</v>
       </c>
       <c r="K71" s="10" t="s">
@@ -2053,8 +2369,8 @@
       <c r="N71" s="12"/>
     </row>
     <row r="72" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I72" s="43"/>
-      <c r="J72" s="46"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="56"/>
       <c r="K72" s="4" t="s">
         <v>36</v>
       </c>
@@ -2065,8 +2381,8 @@
       <c r="N72" s="6"/>
     </row>
     <row r="73" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I73" s="43"/>
-      <c r="J73" s="46"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="56"/>
       <c r="K73" s="4" t="s">
         <v>37</v>
       </c>
@@ -2077,8 +2393,8 @@
       <c r="N73" s="6"/>
     </row>
     <row r="74" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I74" s="53"/>
-      <c r="J74" s="55"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="61"/>
       <c r="K74" s="8" t="s">
         <v>38</v>
       </c>
@@ -2089,13 +2405,13 @@
       <c r="N74" s="9"/>
     </row>
     <row r="75" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="I75" s="42">
+      <c r="I75" s="62">
         <v>12</v>
       </c>
-      <c r="J75" s="45" t="s">
+      <c r="J75" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="K75" s="48" t="s">
+      <c r="K75" s="66" t="s">
         <v>42</v>
       </c>
       <c r="L75" s="32" t="s">
@@ -2105,9 +2421,9 @@
       <c r="N75" s="14"/>
     </row>
     <row r="76" spans="9:14" x14ac:dyDescent="0.2">
-      <c r="I76" s="43"/>
-      <c r="J76" s="46"/>
-      <c r="K76" s="49"/>
+      <c r="I76" s="53"/>
+      <c r="J76" s="56"/>
+      <c r="K76" s="48"/>
       <c r="L76" s="33" t="s">
         <v>10</v>
       </c>
@@ -2115,9 +2431,9 @@
       <c r="N76" s="6"/>
     </row>
     <row r="77" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="44"/>
-      <c r="J77" s="47"/>
-      <c r="K77" s="50"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="65"/>
+      <c r="K77" s="67"/>
       <c r="L77" s="34" t="s">
         <v>11</v>
       </c>
@@ -2127,24 +2443,6 @@
     <row r="78" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="I17:I23"/>
-    <mergeCell ref="J17:J23"/>
-    <mergeCell ref="I24:I31"/>
-    <mergeCell ref="J24:J31"/>
-    <mergeCell ref="J38:J43"/>
-    <mergeCell ref="I55:I60"/>
-    <mergeCell ref="J55:J60"/>
-    <mergeCell ref="I67:I70"/>
-    <mergeCell ref="J67:J70"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="J52:J54"/>
-    <mergeCell ref="I61:I66"/>
-    <mergeCell ref="J61:J66"/>
     <mergeCell ref="I75:I77"/>
     <mergeCell ref="J75:J77"/>
     <mergeCell ref="K75:K77"/>
@@ -2161,8 +2459,1008 @@
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="J32:J37"/>
     <mergeCell ref="I38:I43"/>
+    <mergeCell ref="J38:J43"/>
+    <mergeCell ref="I55:I60"/>
+    <mergeCell ref="J55:J60"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="J52:J54"/>
+    <mergeCell ref="I61:I66"/>
+    <mergeCell ref="J61:J66"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="I17:I23"/>
+    <mergeCell ref="J17:J23"/>
+    <mergeCell ref="I24:I31"/>
+    <mergeCell ref="J24:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F9:K82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="63.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="6:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="52">
+        <v>1</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="72">
+        <v>1</v>
+      </c>
+      <c r="K11" s="73"/>
+    </row>
+    <row r="12" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F12" s="53"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="74"/>
+      <c r="K12" s="75"/>
+    </row>
+    <row r="13" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F13" s="53"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="74"/>
+      <c r="K13" s="75"/>
+    </row>
+    <row r="14" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F14" s="53"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="74"/>
+      <c r="K14" s="75"/>
+    </row>
+    <row r="15" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F15" s="53"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="74"/>
+      <c r="K15" s="75"/>
+    </row>
+    <row r="16" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F16" s="53"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="74"/>
+      <c r="K16" s="75"/>
+    </row>
+    <row r="17" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="54"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="77"/>
+      <c r="K17" s="78"/>
+    </row>
+    <row r="18" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="58">
+        <v>2</v>
+      </c>
+      <c r="G18" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="79" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="122">
+        <v>1</v>
+      </c>
+      <c r="K18" s="124"/>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F19" s="53"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="K19" s="125" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F20" s="53"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="125" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F21" s="53"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="123">
+        <v>0</v>
+      </c>
+      <c r="K21" s="125" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F22" s="53"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="123">
+        <v>1</v>
+      </c>
+      <c r="K22" s="125"/>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F23" s="53"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="123">
+        <v>1</v>
+      </c>
+      <c r="K23" s="125"/>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F24" s="53"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="123">
+        <v>0.9</v>
+      </c>
+      <c r="K24" s="125"/>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F25" s="53"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="123">
+        <v>0.6</v>
+      </c>
+      <c r="K25" s="125"/>
+    </row>
+    <row r="26" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="59"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="127">
+        <v>1</v>
+      </c>
+      <c r="K26" s="126"/>
+    </row>
+    <row r="27" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="82">
+        <v>3</v>
+      </c>
+      <c r="G27" s="83" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="83"/>
+      <c r="K27" s="86"/>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F28" s="87"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="88"/>
+      <c r="K28" s="91"/>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F29" s="87"/>
+      <c r="G29" s="88"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="88"/>
+      <c r="K29" s="91"/>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F30" s="87"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="88"/>
+      <c r="K30" s="91"/>
+    </row>
+    <row r="31" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F31" s="87"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="88"/>
+      <c r="K31" s="91"/>
+    </row>
+    <row r="32" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="93"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="94"/>
+      <c r="K32" s="97"/>
+    </row>
+    <row r="33" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="82">
+        <v>4</v>
+      </c>
+      <c r="G33" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="83"/>
+      <c r="K33" s="86"/>
+    </row>
+    <row r="34" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F34" s="87"/>
+      <c r="G34" s="88"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="88"/>
+      <c r="K34" s="91"/>
+    </row>
+    <row r="35" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F35" s="87"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="I35" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="88"/>
+      <c r="K35" s="91"/>
+    </row>
+    <row r="36" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F36" s="87"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="88"/>
+      <c r="K36" s="91"/>
+    </row>
+    <row r="37" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F37" s="87"/>
+      <c r="G37" s="88"/>
+      <c r="H37" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="88"/>
+      <c r="K37" s="91"/>
+    </row>
+    <row r="38" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="102" t="s">
+        <v>75</v>
+      </c>
+      <c r="I38" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="101"/>
+      <c r="K38" s="104"/>
+    </row>
+    <row r="39" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F39" s="105">
+        <v>5</v>
+      </c>
+      <c r="G39" s="106" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="108" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="106"/>
+      <c r="K39" s="109"/>
+    </row>
+    <row r="40" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F40" s="87"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" s="88"/>
+      <c r="K40" s="91"/>
+    </row>
+    <row r="41" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F41" s="87"/>
+      <c r="G41" s="88"/>
+      <c r="H41" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="90"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="91"/>
+    </row>
+    <row r="42" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F42" s="87"/>
+      <c r="G42" s="88"/>
+      <c r="H42" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="88"/>
+      <c r="K42" s="91"/>
+    </row>
+    <row r="43" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F43" s="87"/>
+      <c r="G43" s="88"/>
+      <c r="H43" s="92" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="88"/>
+      <c r="K43" s="91"/>
+    </row>
+    <row r="44" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="93"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="95" t="s">
+        <v>79</v>
+      </c>
+      <c r="I44" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="94"/>
+      <c r="K44" s="97"/>
+    </row>
+    <row r="45" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F45" s="82">
+        <v>6</v>
+      </c>
+      <c r="G45" s="83" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="110" t="s">
+        <v>81</v>
+      </c>
+      <c r="I45" s="85"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="86"/>
+    </row>
+    <row r="46" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F46" s="87"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="88"/>
+      <c r="K46" s="91"/>
+    </row>
+    <row r="47" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F47" s="87"/>
+      <c r="G47" s="88"/>
+      <c r="H47" s="92" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="88"/>
+      <c r="K47" s="91"/>
+    </row>
+    <row r="48" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F48" s="87"/>
+      <c r="G48" s="88"/>
+      <c r="H48" s="92" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="88"/>
+      <c r="K48" s="91"/>
+    </row>
+    <row r="49" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F49" s="87"/>
+      <c r="G49" s="88"/>
+      <c r="H49" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="I49" s="90"/>
+      <c r="J49" s="88"/>
+      <c r="K49" s="91"/>
+    </row>
+    <row r="50" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="100"/>
+      <c r="G50" s="101"/>
+      <c r="H50" s="102" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="101"/>
+      <c r="K50" s="104"/>
+    </row>
+    <row r="51" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F51" s="105">
+        <v>7</v>
+      </c>
+      <c r="G51" s="106" t="s">
+        <v>58</v>
+      </c>
+      <c r="H51" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" s="108"/>
+      <c r="J51" s="106"/>
+      <c r="K51" s="109"/>
+    </row>
+    <row r="52" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F52" s="87"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="I52" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" s="88"/>
+      <c r="K52" s="91"/>
+    </row>
+    <row r="53" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F53" s="87"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="I53" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J53" s="88"/>
+      <c r="K53" s="91"/>
+    </row>
+    <row r="54" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F54" s="87"/>
+      <c r="G54" s="88"/>
+      <c r="H54" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J54" s="88"/>
+      <c r="K54" s="91"/>
+    </row>
+    <row r="55" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F55" s="87"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I55" s="90"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="91"/>
+    </row>
+    <row r="56" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="93"/>
+      <c r="G56" s="94"/>
+      <c r="H56" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="I56" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="94"/>
+      <c r="K56" s="97"/>
+    </row>
+    <row r="57" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F57" s="82">
+        <v>8</v>
+      </c>
+      <c r="G57" s="83" t="s">
+        <v>59</v>
+      </c>
+      <c r="H57" s="113" t="s">
+        <v>81</v>
+      </c>
+      <c r="I57" s="85"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="86"/>
+    </row>
+    <row r="58" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F58" s="87"/>
+      <c r="G58" s="88"/>
+      <c r="H58" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="114" t="s">
+        <v>10</v>
+      </c>
+      <c r="J58" s="88"/>
+      <c r="K58" s="91"/>
+    </row>
+    <row r="59" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F59" s="87"/>
+      <c r="G59" s="88"/>
+      <c r="H59" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="I59" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" s="88"/>
+      <c r="K59" s="91"/>
+    </row>
+    <row r="60" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F60" s="87"/>
+      <c r="G60" s="88"/>
+      <c r="H60" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I60" s="90"/>
+      <c r="J60" s="88"/>
+      <c r="K60" s="91"/>
+    </row>
+    <row r="61" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="100"/>
+      <c r="G61" s="101"/>
+      <c r="H61" s="102" t="s">
+        <v>86</v>
+      </c>
+      <c r="I61" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" s="101"/>
+      <c r="K61" s="104"/>
+    </row>
+    <row r="62" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F62" s="105">
+        <v>9</v>
+      </c>
+      <c r="G62" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="H62" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="I62" s="85"/>
+      <c r="J62" s="106"/>
+      <c r="K62" s="109"/>
+    </row>
+    <row r="63" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F63" s="87"/>
+      <c r="G63" s="88"/>
+      <c r="H63" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="114" t="s">
+        <v>10</v>
+      </c>
+      <c r="J63" s="88"/>
+      <c r="K63" s="91"/>
+    </row>
+    <row r="64" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F64" s="87"/>
+      <c r="G64" s="88"/>
+      <c r="H64" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="88"/>
+      <c r="K64" s="91"/>
+    </row>
+    <row r="65" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F65" s="87"/>
+      <c r="G65" s="88"/>
+      <c r="H65" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I65" s="90"/>
+      <c r="J65" s="88"/>
+      <c r="K65" s="91"/>
+    </row>
+    <row r="66" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="93"/>
+      <c r="G66" s="94"/>
+      <c r="H66" s="95" t="s">
+        <v>87</v>
+      </c>
+      <c r="I66" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J66" s="94"/>
+      <c r="K66" s="97"/>
+    </row>
+    <row r="67" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F67" s="82">
+        <v>10</v>
+      </c>
+      <c r="G67" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" s="113" t="s">
+        <v>81</v>
+      </c>
+      <c r="I67" s="85"/>
+      <c r="J67" s="83"/>
+      <c r="K67" s="86"/>
+    </row>
+    <row r="68" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F68" s="87"/>
+      <c r="G68" s="88"/>
+      <c r="H68" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="I68" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J68" s="88"/>
+      <c r="K68" s="91"/>
+    </row>
+    <row r="69" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F69" s="87"/>
+      <c r="G69" s="88"/>
+      <c r="H69" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="I69" s="114" t="s">
+        <v>10</v>
+      </c>
+      <c r="J69" s="88"/>
+      <c r="K69" s="91"/>
+    </row>
+    <row r="70" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F70" s="87"/>
+      <c r="G70" s="88"/>
+      <c r="H70" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I70" s="90"/>
+      <c r="J70" s="88"/>
+      <c r="K70" s="91"/>
+    </row>
+    <row r="71" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F71" s="100"/>
+      <c r="G71" s="101"/>
+      <c r="H71" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="I71" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J71" s="101"/>
+      <c r="K71" s="104"/>
+    </row>
+    <row r="72" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F72" s="105">
+        <v>11</v>
+      </c>
+      <c r="G72" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="I72" s="108"/>
+      <c r="J72" s="106"/>
+      <c r="K72" s="109"/>
+    </row>
+    <row r="73" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F73" s="87"/>
+      <c r="G73" s="88"/>
+      <c r="H73" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="I73" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J73" s="88"/>
+      <c r="K73" s="91"/>
+    </row>
+    <row r="74" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F74" s="87"/>
+      <c r="G74" s="88"/>
+      <c r="H74" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="I74" s="114" t="s">
+        <v>10</v>
+      </c>
+      <c r="J74" s="88"/>
+      <c r="K74" s="91"/>
+    </row>
+    <row r="75" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F75" s="87"/>
+      <c r="G75" s="88"/>
+      <c r="H75" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I75" s="90"/>
+      <c r="J75" s="88"/>
+      <c r="K75" s="91"/>
+    </row>
+    <row r="76" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F76" s="93"/>
+      <c r="G76" s="94"/>
+      <c r="H76" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="I76" s="96" t="s">
+        <v>7</v>
+      </c>
+      <c r="J76" s="94"/>
+      <c r="K76" s="97"/>
+    </row>
+    <row r="77" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F77" s="82">
+        <v>12</v>
+      </c>
+      <c r="G77" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="H77" s="113" t="s">
+        <v>81</v>
+      </c>
+      <c r="I77" s="85"/>
+      <c r="J77" s="83"/>
+      <c r="K77" s="86"/>
+    </row>
+    <row r="78" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F78" s="87"/>
+      <c r="G78" s="88"/>
+      <c r="H78" s="115" t="s">
+        <v>39</v>
+      </c>
+      <c r="I78" s="114" t="s">
+        <v>10</v>
+      </c>
+      <c r="J78" s="88"/>
+      <c r="K78" s="91"/>
+    </row>
+    <row r="79" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F79" s="87"/>
+      <c r="G79" s="88"/>
+      <c r="H79" s="116"/>
+      <c r="I79" s="114" t="s">
+        <v>11</v>
+      </c>
+      <c r="J79" s="88"/>
+      <c r="K79" s="91"/>
+    </row>
+    <row r="80" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F80" s="87"/>
+      <c r="G80" s="88"/>
+      <c r="H80" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="I80" s="90"/>
+      <c r="J80" s="88"/>
+      <c r="K80" s="91"/>
+    </row>
+    <row r="81" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F81" s="117"/>
+      <c r="G81" s="118"/>
+      <c r="H81" s="119" t="s">
+        <v>93</v>
+      </c>
+      <c r="I81" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" s="118"/>
+      <c r="K81" s="121"/>
+    </row>
+    <row r="82" spans="6:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="51">
+    <mergeCell ref="F72:F76"/>
+    <mergeCell ref="G72:G76"/>
+    <mergeCell ref="J72:J76"/>
+    <mergeCell ref="K72:K76"/>
+    <mergeCell ref="F77:F81"/>
+    <mergeCell ref="G77:G81"/>
+    <mergeCell ref="J77:J81"/>
+    <mergeCell ref="K77:K81"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="F62:F66"/>
+    <mergeCell ref="G62:G66"/>
+    <mergeCell ref="J62:J66"/>
+    <mergeCell ref="K62:K66"/>
+    <mergeCell ref="F67:F71"/>
+    <mergeCell ref="G67:G71"/>
+    <mergeCell ref="J67:J71"/>
+    <mergeCell ref="K67:K71"/>
+    <mergeCell ref="F51:F56"/>
+    <mergeCell ref="G51:G56"/>
+    <mergeCell ref="J51:J56"/>
+    <mergeCell ref="K51:K56"/>
+    <mergeCell ref="F57:F61"/>
+    <mergeCell ref="G57:G61"/>
+    <mergeCell ref="J57:J61"/>
+    <mergeCell ref="K57:K61"/>
+    <mergeCell ref="F39:F44"/>
+    <mergeCell ref="G39:G44"/>
+    <mergeCell ref="J39:J44"/>
+    <mergeCell ref="K39:K44"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="J45:J50"/>
+    <mergeCell ref="K45:K50"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="K27:K32"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="J33:J38"/>
+    <mergeCell ref="K33:K38"/>
+    <mergeCell ref="F11:F17"/>
+    <mergeCell ref="G11:G17"/>
+    <mergeCell ref="J11:J17"/>
+    <mergeCell ref="K11:K17"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F18:F26"/>
+    <mergeCell ref="G18:G26"/>
+    <mergeCell ref="H23:H25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>